<commit_message>
Upload files to console based on cn181107
</commit_message>
<xml_diff>
--- a/console/Networking/networkExcel1029/componentsMixinsXlsx/elasticNetworkMixinsXlsx/multipleIpInput.xlsx
+++ b/console/Networking/networkExcel1029/componentsMixinsXlsx/elasticNetworkMixinsXlsx/multipleIpInput.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhaoxiangyi\Desktop\11.1\2018.11.1 京东云console-精益通-韩凯\质检-1810-31_HO_console-译文-提交\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\han\Desktop\京东云-返工\20. 弹性网卡控制台国际化翻译校对\3. 客户确认版-更新至github\弹性网卡确认-GTCOM-haopeng1108-需更新至github\componentsMixinsXlsx_elasticNetworkMixinsXlsx_haopeng1106-R\elasticNetworkMixinsXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="ch" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -137,18 +137,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>新增一行</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>multipleIpInput_i18nKey_6</t>
     </r>
   </si>
@@ -161,18 +149,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">'自动分配' </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>multipleIpInput_i18nKey_7</t>
     </r>
   </si>
@@ -389,54 +365,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>If customization is selected, please</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Designated within Section</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Add a new row</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">'Automatic Allocate' </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">'Customized' </t>
     </r>
   </si>
@@ -449,18 +377,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>'IP address has been already assigned'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>'Please enter a valid IP address'</t>
     </r>
   </si>
@@ -473,55 +389,79 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>'Please enter different IP address'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'This IP address is not'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>''Within or has been reserved';'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>'IP address will be assigned automatically'</t>
     </r>
   </si>
   <si>
-    <t>IP address has already been assigned</t>
+    <t>Auto Assign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assign new IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Please enter another IP address since this IP address has been already assigned.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>自动分配</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">' </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增一行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Please enter a different IP address'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If customization is selected, please</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>specify the IP address in the range of " ".</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This IP address has been already assigned.'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>" " or has been reserved.'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'This IP address is out of the range of '</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -531,6 +471,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="3"/>
       <charset val="134"/>
@@ -557,8 +505,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -900,13 +850,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.44140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="44.109375" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -917,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -928,10 +878,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -939,7 +889,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -950,124 +900,125 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" s="2" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
+      <c r="C12" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B14" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B4 A7:B14 A6 A5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>